<commit_message>
median JanJul konstanty submission sub_13 - sub17
</commit_message>
<xml_diff>
--- a/Excely/mean median pomocne.xlsx
+++ b/Excely/mean median pomocne.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>MEANS</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t xml:space="preserve">whole </t>
+  </si>
+  <si>
+    <t>Medians</t>
   </si>
 </sst>
 </file>
@@ -270,11 +273,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="366635112"/>
-        <c:axId val="366639424"/>
+        <c:axId val="363859784"/>
+        <c:axId val="363857432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="366635112"/>
+        <c:axId val="363859784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -331,12 +334,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366639424"/>
+        <c:crossAx val="363857432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="366639424"/>
+        <c:axId val="363857432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -393,7 +396,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366635112"/>
+        <c:crossAx val="363859784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1328,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,6 +1441,105 @@
         <v>1.0000337719803942</v>
       </c>
     </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2013</v>
+      </c>
+      <c r="B21">
+        <v>6814.3919999999998</v>
+      </c>
+      <c r="C21">
+        <v>6147</v>
+      </c>
+      <c r="D21">
+        <v>5960.5</v>
+      </c>
+      <c r="F21">
+        <f>D21/C21</f>
+        <v>0.96965999674638037</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2014</v>
+      </c>
+      <c r="B22">
+        <v>7025.4040000000005</v>
+      </c>
+      <c r="C22">
+        <v>6301</v>
+      </c>
+      <c r="D22">
+        <v>6186</v>
+      </c>
+      <c r="F22">
+        <f>D22/C22</f>
+        <v>0.98174892874146957</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2015</v>
+      </c>
+      <c r="B23">
+        <v>7088.1270000000004</v>
+      </c>
+      <c r="C23">
+        <v>6530</v>
+      </c>
+      <c r="D23" s="1">
+        <f>C23*F23</f>
+        <v>6371.3501417178304</v>
+      </c>
+      <c r="F23">
+        <f>(F22+F21)/2</f>
+        <v>0.97570446274392497</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <f>AVERAGE(C21:C23)</f>
+        <v>6326</v>
+      </c>
+      <c r="D25">
+        <v>6371.3501417178304</v>
+      </c>
+      <c r="F25">
+        <f>D25/C25</f>
+        <v>1.0071688494653541</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>6889.3403333333335</v>
+      </c>
+      <c r="D31">
+        <v>6889.5730000000003</v>
+      </c>
+      <c r="F31">
+        <f>D31/C31</f>
+        <v>1.0000337719803942</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>